<commit_message>
Bugfix: Send E-mails fixed
</commit_message>
<xml_diff>
--- a/BD_Ass.xlsx
+++ b/BD_Ass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicor\OneDrive\Desktop\Ass de e-mail Auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FB5CD1-C7D0-41FC-B0E8-FF64352040E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF93083-21D9-4E08-AA22-BDBBA85E8E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9B1777C8-B27A-4E82-A88F-016067786B88}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9B1777C8-B27A-4E82-A88F-016067786B88}"/>
   </bookViews>
   <sheets>
     <sheet name="Assinaturas_Format" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="193">
   <si>
     <t>NOME COMPLETO</t>
   </si>
@@ -69,21 +69,12 @@
     <t>TELEFONE FORMATADO</t>
   </si>
   <si>
-    <t>Silva</t>
-  </si>
-  <si>
-    <t>José</t>
-  </si>
-  <si>
     <t>Departamento Pessoal</t>
   </si>
   <si>
     <t>Marketing</t>
   </si>
   <si>
-    <t>Ana</t>
-  </si>
-  <si>
     <t>Guilherme Gama</t>
   </si>
   <si>
@@ -456,180 +447,12 @@
     <t>Diego Martins</t>
   </si>
   <si>
-    <t>97241</t>
-  </si>
-  <si>
-    <t>9431</t>
-  </si>
-  <si>
-    <t>97241-9431</t>
-  </si>
-  <si>
-    <t>Guilherme</t>
-  </si>
-  <si>
-    <t>Gama</t>
-  </si>
-  <si>
-    <t>99914</t>
-  </si>
-  <si>
-    <t>4871</t>
-  </si>
-  <si>
-    <t>99914-4871</t>
-  </si>
-  <si>
-    <t>Nicolas</t>
-  </si>
-  <si>
-    <t>Reis</t>
-  </si>
-  <si>
-    <t>95916</t>
-  </si>
-  <si>
-    <t>1780</t>
-  </si>
-  <si>
-    <t>95916-1780</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Pinheiro</t>
-  </si>
-  <si>
-    <t>99684</t>
-  </si>
-  <si>
-    <t>1186</t>
-  </si>
-  <si>
-    <t>99684-1186</t>
-  </si>
-  <si>
-    <t>Antonio</t>
-  </si>
-  <si>
-    <t>Macedo</t>
-  </si>
-  <si>
-    <t>95023</t>
-  </si>
-  <si>
-    <t>5577</t>
-  </si>
-  <si>
-    <t>95023-5577</t>
-  </si>
-  <si>
-    <t>Eduardo</t>
-  </si>
-  <si>
-    <t>95145</t>
-  </si>
-  <si>
-    <t>2676</t>
-  </si>
-  <si>
-    <t>95145-2676</t>
-  </si>
-  <si>
-    <t>Mirella</t>
-  </si>
-  <si>
-    <t>Fernandes</t>
-  </si>
-  <si>
-    <t>98149</t>
-  </si>
-  <si>
-    <t>2589</t>
-  </si>
-  <si>
-    <t>98149-2589</t>
-  </si>
-  <si>
-    <t>Vitor</t>
-  </si>
-  <si>
-    <t>Junquetti</t>
-  </si>
-  <si>
-    <t>96705</t>
-  </si>
-  <si>
-    <t>2587</t>
-  </si>
-  <si>
-    <t>96705-2587</t>
-  </si>
-  <si>
-    <t>Rafaella</t>
-  </si>
-  <si>
-    <t>Beneton</t>
-  </si>
-  <si>
-    <t>99988</t>
-  </si>
-  <si>
-    <t>0789</t>
-  </si>
-  <si>
-    <t>99988-0789</t>
-  </si>
-  <si>
-    <t>Juvenal</t>
-  </si>
-  <si>
     <t>Alves</t>
   </si>
   <si>
-    <t>99117</t>
-  </si>
-  <si>
-    <t>4369</t>
-  </si>
-  <si>
-    <t>99117-4369</t>
-  </si>
-  <si>
-    <t>Debora</t>
-  </si>
-  <si>
     <t>Rodrigues</t>
   </si>
   <si>
-    <t>99907</t>
-  </si>
-  <si>
-    <t>2983</t>
-  </si>
-  <si>
-    <t>99907-2983</t>
-  </si>
-  <si>
-    <t>Adriano</t>
-  </si>
-  <si>
-    <t>Carvalho</t>
-  </si>
-  <si>
-    <t>99715</t>
-  </si>
-  <si>
-    <t>1148</t>
-  </si>
-  <si>
-    <t>99715-1148</t>
-  </si>
-  <si>
-    <t>Mateus</t>
-  </si>
-  <si>
     <t>99918</t>
   </si>
   <si>
@@ -642,492 +465,9 @@
     <t>Isis</t>
   </si>
   <si>
-    <t>Gomes</t>
-  </si>
-  <si>
-    <t>98497</t>
-  </si>
-  <si>
-    <t>5415</t>
-  </si>
-  <si>
-    <t>98497-5415</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
-    <t>98422</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>98422-2012</t>
-  </si>
-  <si>
-    <t>Bruna</t>
-  </si>
-  <si>
-    <t>Copa</t>
-  </si>
-  <si>
-    <t>94571</t>
-  </si>
-  <si>
-    <t>3582</t>
-  </si>
-  <si>
-    <t>94571-3582</t>
-  </si>
-  <si>
-    <t>Bárbara</t>
-  </si>
-  <si>
-    <t>Massani</t>
-  </si>
-  <si>
-    <t>94782</t>
-  </si>
-  <si>
-    <t>7339</t>
-  </si>
-  <si>
-    <t>94782-7339</t>
-  </si>
-  <si>
-    <t>Basso</t>
-  </si>
-  <si>
-    <t>99138</t>
-  </si>
-  <si>
-    <t>3407</t>
-  </si>
-  <si>
-    <t>99138-3407</t>
-  </si>
-  <si>
-    <t>Haryany</t>
-  </si>
-  <si>
-    <t>Oliveira</t>
-  </si>
-  <si>
-    <t>95055</t>
-  </si>
-  <si>
-    <t>3939</t>
-  </si>
-  <si>
-    <t>95055-3939</t>
-  </si>
-  <si>
-    <t>Pamella</t>
-  </si>
-  <si>
-    <t>Morão</t>
-  </si>
-  <si>
-    <t>98160</t>
-  </si>
-  <si>
-    <t>1876</t>
-  </si>
-  <si>
-    <t>98160-1876</t>
-  </si>
-  <si>
-    <t>Lima</t>
-  </si>
-  <si>
-    <t>95979</t>
-  </si>
-  <si>
-    <t>3172</t>
-  </si>
-  <si>
-    <t>95979-3172</t>
-  </si>
-  <si>
-    <t>Vanessa</t>
-  </si>
-  <si>
     <t>Cardoso</t>
   </si>
   <si>
-    <t>99848</t>
-  </si>
-  <si>
-    <t>9247</t>
-  </si>
-  <si>
-    <t>99848-9247</t>
-  </si>
-  <si>
-    <t>Felipe</t>
-  </si>
-  <si>
-    <t>97682</t>
-  </si>
-  <si>
-    <t>9954</t>
-  </si>
-  <si>
-    <t>97682-9954</t>
-  </si>
-  <si>
-    <t>Gilmar</t>
-  </si>
-  <si>
-    <t>Herculano</t>
-  </si>
-  <si>
-    <t>96840</t>
-  </si>
-  <si>
-    <t>7080</t>
-  </si>
-  <si>
-    <t>96840-7080</t>
-  </si>
-  <si>
-    <t>Marina</t>
-  </si>
-  <si>
-    <t>Corral</t>
-  </si>
-  <si>
-    <t>99416</t>
-  </si>
-  <si>
-    <t>9207</t>
-  </si>
-  <si>
-    <t>99416-9207</t>
-  </si>
-  <si>
-    <t>Paulo</t>
-  </si>
-  <si>
-    <t>Roso</t>
-  </si>
-  <si>
-    <t>99953</t>
-  </si>
-  <si>
-    <t>5484</t>
-  </si>
-  <si>
-    <t>99953-5484</t>
-  </si>
-  <si>
-    <t>Andrey</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>98835</t>
-  </si>
-  <si>
-    <t>6360</t>
-  </si>
-  <si>
-    <t>98835-6360</t>
-  </si>
-  <si>
-    <t>Brenda</t>
-  </si>
-  <si>
-    <t>Ferreira</t>
-  </si>
-  <si>
-    <t>98028</t>
-  </si>
-  <si>
-    <t>8199</t>
-  </si>
-  <si>
-    <t>98028-8199</t>
-  </si>
-  <si>
-    <t>Laís</t>
-  </si>
-  <si>
-    <t>Melo</t>
-  </si>
-  <si>
-    <t>98784</t>
-  </si>
-  <si>
-    <t>6236</t>
-  </si>
-  <si>
-    <t>98784-6236</t>
-  </si>
-  <si>
-    <t>Victória</t>
-  </si>
-  <si>
-    <t>Carneiro</t>
-  </si>
-  <si>
-    <t>96922</t>
-  </si>
-  <si>
-    <t>0331</t>
-  </si>
-  <si>
-    <t>96922-0331</t>
-  </si>
-  <si>
-    <t>Gabriela</t>
-  </si>
-  <si>
-    <t>97012</t>
-  </si>
-  <si>
-    <t>0282</t>
-  </si>
-  <si>
-    <t>97012-0282</t>
-  </si>
-  <si>
-    <t>Luana</t>
-  </si>
-  <si>
-    <t>Maranho</t>
-  </si>
-  <si>
-    <t>99726</t>
-  </si>
-  <si>
-    <t>1787</t>
-  </si>
-  <si>
-    <t>99726-1787</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>99960</t>
-  </si>
-  <si>
-    <t>6361</t>
-  </si>
-  <si>
-    <t>99960-6361</t>
-  </si>
-  <si>
-    <t>Viviane</t>
-  </si>
-  <si>
-    <t>Pizzo</t>
-  </si>
-  <si>
-    <t>99968</t>
-  </si>
-  <si>
-    <t>6392</t>
-  </si>
-  <si>
-    <t>99968-6392</t>
-  </si>
-  <si>
-    <t>Maurici</t>
-  </si>
-  <si>
-    <t>Cunha</t>
-  </si>
-  <si>
-    <t>98872</t>
-  </si>
-  <si>
-    <t>7603</t>
-  </si>
-  <si>
-    <t>98872-7603</t>
-  </si>
-  <si>
-    <t>Nathalia</t>
-  </si>
-  <si>
-    <t>Araujo</t>
-  </si>
-  <si>
-    <t>96285</t>
-  </si>
-  <si>
-    <t>4697</t>
-  </si>
-  <si>
-    <t>96285-4697</t>
-  </si>
-  <si>
-    <t>Joyce</t>
-  </si>
-  <si>
-    <t>Ambrosio</t>
-  </si>
-  <si>
-    <t>99333</t>
-  </si>
-  <si>
-    <t>2993</t>
-  </si>
-  <si>
-    <t>99333-2993</t>
-  </si>
-  <si>
-    <t>Sabrina</t>
-  </si>
-  <si>
-    <t>96508</t>
-  </si>
-  <si>
-    <t>4725</t>
-  </si>
-  <si>
-    <t>96508-4725</t>
-  </si>
-  <si>
-    <t>Neto</t>
-  </si>
-  <si>
-    <t>94706</t>
-  </si>
-  <si>
-    <t>8443</t>
-  </si>
-  <si>
-    <t>94706-8443</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Barbaro</t>
-  </si>
-  <si>
-    <t>98660</t>
-  </si>
-  <si>
-    <t>9142</t>
-  </si>
-  <si>
-    <t>98660-9142</t>
-  </si>
-  <si>
-    <t>André</t>
-  </si>
-  <si>
-    <t>Nogueira</t>
-  </si>
-  <si>
-    <t>96428</t>
-  </si>
-  <si>
-    <t>2924</t>
-  </si>
-  <si>
-    <t>96428-2924</t>
-  </si>
-  <si>
-    <t>Jardel</t>
-  </si>
-  <si>
-    <t>Santos</t>
-  </si>
-  <si>
-    <t>95025</t>
-  </si>
-  <si>
-    <t>3020</t>
-  </si>
-  <si>
-    <t>95025-3020</t>
-  </si>
-  <si>
-    <t>Kémilly</t>
-  </si>
-  <si>
-    <t>Brito</t>
-  </si>
-  <si>
-    <t>94904</t>
-  </si>
-  <si>
-    <t>5917</t>
-  </si>
-  <si>
-    <t>94904-5917</t>
-  </si>
-  <si>
-    <t>Menezes</t>
-  </si>
-  <si>
-    <t>94014</t>
-  </si>
-  <si>
-    <t>2242</t>
-  </si>
-  <si>
-    <t>94014-2242</t>
-  </si>
-  <si>
-    <t>Gabriel</t>
-  </si>
-  <si>
-    <t>97231</t>
-  </si>
-  <si>
-    <t>1129</t>
-  </si>
-  <si>
-    <t>97231-1129</t>
-  </si>
-  <si>
-    <t>Homero</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>94760</t>
-  </si>
-  <si>
-    <t>7963</t>
-  </si>
-  <si>
-    <t>94760-7963</t>
-  </si>
-  <si>
-    <t>Marcio</t>
-  </si>
-  <si>
-    <t>95177</t>
-  </si>
-  <si>
-    <t>4496</t>
-  </si>
-  <si>
-    <t>95177-4496</t>
-  </si>
-  <si>
-    <t>94068</t>
-  </si>
-  <si>
-    <t>5699</t>
-  </si>
-  <si>
-    <t>94068-5699</t>
-  </si>
-  <si>
-    <t>Adriely</t>
-  </si>
-  <si>
     <t>19276</t>
   </si>
   <si>
@@ -1197,18 +537,6 @@
     <t>Graziani</t>
   </si>
   <si>
-    <t>98259</t>
-  </si>
-  <si>
-    <t>2620</t>
-  </si>
-  <si>
-    <t>98259-2620</t>
-  </si>
-  <si>
-    <t>Kodoma</t>
-  </si>
-  <si>
     <t>94258</t>
   </si>
   <si>
@@ -1254,102 +582,6 @@
     <t>E-MAIL</t>
   </si>
   <si>
-    <t>guilherme.gama@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>nicolas.reis@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>antonio.macedo@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>mirella.fernandes@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>vitor.junquetti@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>rafaella.beneton@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>debora.rodrigues@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>adriano.carvalho@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>mateus.silva@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>george.silva@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>bruna.copa@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>bárbara.massani@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>lucas.basso@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>haryany.oliveira@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>ana.lima@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>vanessa.cardoso@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>felipe.rodrigues@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>gilmar.herculano@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>marina.corral@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>paulo.roso@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>andrey.sales@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>brenda.ferreira@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>gabriela.gomes@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>luana.maranho@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>viviane.pizzo@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>nathalia.araujo@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>joyce.ambrosio@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>maria.barbaro@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>jardel.santos@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>guilherme.menezes@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>gabriel.carneiro@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>homero.junior@unitaengenharia.com.br</t>
-  </si>
-  <si>
     <t>leandro.vieira@unitaengenharia.com.br</t>
   </si>
   <si>
@@ -1365,9 +597,6 @@
     <t>juliana.graziani@unitaengenharia.com.br</t>
   </si>
   <si>
-    <t>gabriela.kodoma@unitaengenharia.com.br</t>
-  </si>
-  <si>
     <t>diego.martins@unitaengenharia.com.br</t>
   </si>
   <si>
@@ -1377,136 +606,19 @@
     <t>renato.rodrigues@unitaengenharia.com.br</t>
   </si>
   <si>
-    <t>lucas@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>eduardo.macedo@unitaengenharia.com.br</t>
-  </si>
-  <si>
     <t>Siilva</t>
   </si>
   <si>
-    <t>isis.siilva@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>pamella.morao@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>lais.melo@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>victória.araujo@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>bruno.paulo@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>maurici@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>sabrina.silva@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>jose.neto@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>andre.nogueira@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>kemilly.brito@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>marcio.oliveira@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>andrey.almeida@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>Marcio Oliveira</t>
-  </si>
-  <si>
-    <t>José Neto</t>
-  </si>
-  <si>
-    <t>Sabrina Silva</t>
-  </si>
-  <si>
-    <t>Bruno Paulo</t>
-  </si>
-  <si>
-    <t>Victória Araujo</t>
-  </si>
-  <si>
-    <t>Paulo Roso</t>
-  </si>
-  <si>
-    <t>Ana Lima</t>
-  </si>
-  <si>
-    <t>Bruna Copa</t>
-  </si>
-  <si>
-    <t>George Silva</t>
-  </si>
-  <si>
     <t>Isis Silva</t>
   </si>
   <si>
-    <t>Juvenal Santos</t>
-  </si>
-  <si>
-    <t>juvenal.santos@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>Eduardo Macedo</t>
-  </si>
-  <si>
-    <t>Almeida</t>
-  </si>
-  <si>
-    <t>adriely.silva@unitaengenharia.com.br</t>
-  </si>
-  <si>
-    <t>Adriely Silva</t>
-  </si>
-  <si>
-    <t>CONTROLE &amp; TI</t>
-  </si>
-  <si>
-    <t>SUPRIMENTOS</t>
-  </si>
-  <si>
     <t>ENGENHARIA</t>
   </si>
   <si>
-    <t>ORÇAMENTOS</t>
-  </si>
-  <si>
-    <t>PLANEJAMENTO E CONTROLE</t>
-  </si>
-  <si>
-    <t>GESTÃO ADMINISTRATIVA</t>
-  </si>
-  <si>
-    <t>GENTE E CULTURA</t>
-  </si>
-  <si>
-    <t>QUALIDADE</t>
-  </si>
-  <si>
     <t>PROJETOS</t>
   </si>
   <si>
-    <t>MARKETING</t>
-  </si>
-  <si>
-    <t>DEPARTAMENTO PESSOAL</t>
-  </si>
-  <si>
-    <t>INCORPORAÇÃO</t>
-  </si>
-  <si>
-    <t>suporte.ti@unitaengenharia.com.br</t>
+    <t>isis.silva@unitaengenharia.com.br</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +739,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2009,15 +1123,15 @@
         <v>7</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>403</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2">
         <v>11</v>
@@ -2035,7 +1149,7 @@
         <v>97241-9431</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H2" s="3" t="str">
         <f>IFERROR(LEFT(A2, FIND(" ", A2)-1), " ")</f>
@@ -2052,10 +1166,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2">
         <v>11</v>
@@ -2073,7 +1187,7 @@
         <v>99914-4871</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H3" s="3" t="str">
         <f t="shared" ref="H3:H59" si="6">IFERROR(LEFT(A3, FIND(" ", A3)-1), " ")</f>
@@ -2090,10 +1204,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2">
         <v>11</v>
@@ -2111,7 +1225,7 @@
         <v>95916-1780</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H4" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2128,10 +1242,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2">
         <v>11</v>
@@ -2149,7 +1263,7 @@
         <v>99684-1186</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H5" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2166,10 +1280,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2">
         <v>11</v>
@@ -2187,7 +1301,7 @@
         <v>95023-5577</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H6" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2204,10 +1318,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2">
         <v>11</v>
@@ -2225,7 +1339,7 @@
         <v>95145-2676</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H7" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2242,10 +1356,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2">
         <v>12</v>
@@ -2263,7 +1377,7 @@
         <v>98149-2589</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H8" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2280,10 +1394,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2">
         <v>11</v>
@@ -2301,7 +1415,7 @@
         <v>96705-2587</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H9" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2318,10 +1432,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2">
         <v>11</v>
@@ -2339,7 +1453,7 @@
         <v>99988-0789</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H10" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2356,10 +1470,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2">
         <v>11</v>
@@ -2377,7 +1491,7 @@
         <v>99117-4369</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H11" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2394,10 +1508,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2">
         <v>11</v>
@@ -2415,7 +1529,7 @@
         <v>99907-2983</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H12" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2432,10 +1546,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2">
         <v>12</v>
@@ -2453,7 +1567,7 @@
         <v>99715-1148</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H13" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2470,10 +1584,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2">
         <v>11</v>
@@ -2491,7 +1605,7 @@
         <v>99918-3753</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H14" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2508,10 +1622,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2">
         <v>11</v>
@@ -2529,7 +1643,7 @@
         <v>98497-5415</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H15" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2546,10 +1660,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2">
         <v>11</v>
@@ -2567,7 +1681,7 @@
         <v>98422-2012</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H16" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2584,10 +1698,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2">
         <v>11</v>
@@ -2605,7 +1719,7 @@
         <v>94571-3582</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H17" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2622,10 +1736,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2">
         <v>11</v>
@@ -2643,7 +1757,7 @@
         <v>94782-7339</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H18" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2660,10 +1774,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2">
         <v>11</v>
@@ -2681,7 +1795,7 @@
         <v>99138-3407</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H19" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2698,10 +1812,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2">
         <v>11</v>
@@ -2719,7 +1833,7 @@
         <v>95055-3939</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H20" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2736,10 +1850,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2">
         <v>19</v>
@@ -2757,7 +1871,7 @@
         <v>98160-1876</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H21" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2774,10 +1888,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C22" s="2">
         <v>11</v>
@@ -2795,7 +1909,7 @@
         <v>95979-3172</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H22" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2812,10 +1926,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" s="2">
         <v>15</v>
@@ -2833,7 +1947,7 @@
         <v>99848-9247</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H23" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2850,10 +1964,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2">
         <v>11</v>
@@ -2871,7 +1985,7 @@
         <v>97682-9954</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H24" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2888,10 +2002,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C25" s="2">
         <v>11</v>
@@ -2909,7 +2023,7 @@
         <v>96840-7080</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H25" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2926,10 +2040,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2">
         <v>11</v>
@@ -2947,7 +2061,7 @@
         <v>99416-9207</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H26" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2964,10 +2078,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2">
         <v>11</v>
@@ -2985,7 +2099,7 @@
         <v>99953-5484</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H27" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3002,10 +2116,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2">
         <v>14</v>
@@ -3023,7 +2137,7 @@
         <v>98835-6360</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H28" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3040,10 +2154,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2">
         <v>11</v>
@@ -3061,7 +2175,7 @@
         <v>98028-8199</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H29" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3078,10 +2192,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2">
         <v>11</v>
@@ -3099,7 +2213,7 @@
         <v>98784-6236</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H30" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3116,10 +2230,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2">
         <v>11</v>
@@ -3137,7 +2251,7 @@
         <v>96922-0331</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H31" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3154,10 +2268,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C32" s="2">
         <v>11</v>
@@ -3175,7 +2289,7 @@
         <v>97012-0282</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H32" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3192,10 +2306,10 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2">
         <v>11</v>
@@ -3213,7 +2327,7 @@
         <v>99726-1787</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H33" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3230,10 +2344,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2">
         <v>11</v>
@@ -3251,7 +2365,7 @@
         <v>99960-6361</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H34" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3268,10 +2382,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2">
         <v>11</v>
@@ -3289,7 +2403,7 @@
         <v>99968-6392</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H35" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3306,10 +2420,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2">
         <v>11</v>
@@ -3327,7 +2441,7 @@
         <v>98872-7603</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H36" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3344,10 +2458,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C37" s="2">
         <v>11</v>
@@ -3365,7 +2479,7 @@
         <v>96285-4697</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H37" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3382,10 +2496,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2">
         <v>11</v>
@@ -3403,7 +2517,7 @@
         <v>99333-2993</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H38" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3420,10 +2534,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" s="2">
         <v>11</v>
@@ -3441,7 +2555,7 @@
         <v>97241-9431</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H39" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3458,10 +2572,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C40" s="2">
         <v>11</v>
@@ -3479,7 +2593,7 @@
         <v>96508-4725</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H40" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3496,10 +2610,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C41" s="2">
         <v>11</v>
@@ -3517,7 +2631,7 @@
         <v>94706-8443</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H41" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3534,10 +2648,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C42" s="2">
         <v>11</v>
@@ -3555,7 +2669,7 @@
         <v>98660-9142</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H42" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3572,10 +2686,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C43" s="2">
         <v>11</v>
@@ -3593,7 +2707,7 @@
         <v>96428-2924</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H43" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3610,10 +2724,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C44" s="2">
         <v>11</v>
@@ -3631,7 +2745,7 @@
         <v>95025-3020</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H44" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3648,10 +2762,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C45" s="2">
         <v>11</v>
@@ -3669,7 +2783,7 @@
         <v>94904-5917</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H45" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3686,10 +2800,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C46" s="2">
         <v>11</v>
@@ -3707,7 +2821,7 @@
         <v>94014-2242</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H46" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3724,10 +2838,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C47" s="2">
         <v>11</v>
@@ -3745,7 +2859,7 @@
         <v>97231-1129</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H47" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3762,10 +2876,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C48" s="2">
         <v>11</v>
@@ -3783,7 +2897,7 @@
         <v>94760-7963</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H48" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3800,10 +2914,10 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C49" s="2">
         <v>11</v>
@@ -3821,7 +2935,7 @@
         <v>95177-4496</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H49" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3838,10 +2952,10 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C50" s="2">
         <v>11</v>
@@ -3859,7 +2973,7 @@
         <v>94068-5699</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H50" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3876,10 +2990,10 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C51" s="2">
         <v>31</v>
@@ -3897,7 +3011,7 @@
         <v>19276-2121</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H51" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3914,10 +3028,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C52" s="2">
         <v>11</v>
@@ -3935,7 +3049,7 @@
         <v>98104-9890</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H52" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3952,10 +3066,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C53" s="2">
         <v>11</v>
@@ -3973,7 +3087,7 @@
         <v>98016-2327</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H53" s="3" t="str">
         <f t="shared" si="6"/>
@@ -3990,10 +3104,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C54" s="2">
         <v>11</v>
@@ -4011,7 +3125,7 @@
         <v>97758-4510</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H54" s="3" t="str">
         <f t="shared" si="6"/>
@@ -4028,10 +3142,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C55" s="2">
         <v>11</v>
@@ -4049,7 +3163,7 @@
         <v>97833-1146</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H55" s="3" t="str">
         <f t="shared" si="6"/>
@@ -4066,10 +3180,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C56" s="2">
         <v>11</v>
@@ -4087,7 +3201,7 @@
         <v>98259-2620</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H56" s="3" t="str">
         <f t="shared" si="6"/>
@@ -4104,10 +3218,10 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C57" s="2">
         <v>11</v>
@@ -4125,7 +3239,7 @@
         <v>94258-2007</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H57" s="3" t="str">
         <f t="shared" si="6"/>
@@ -4142,10 +3256,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C58" s="2">
         <v>11</v>
@@ -4163,7 +3277,7 @@
         <v>98484-1118</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H58" s="3" t="str">
         <f t="shared" si="6"/>
@@ -4180,11 +3294,11 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C59" s="2">
         <v>11</v>
       </c>
@@ -4201,7 +3315,7 @@
         <v>96352-9560</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H59" s="3" t="str">
         <f t="shared" si="6"/>
@@ -4225,10 +3339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA79D605-B120-48E8-BCEE-C9DA726CFECB}">
-  <dimension ref="A1:P1439"/>
+  <dimension ref="A1:J1391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4242,9 +3356,10 @@
     <col min="8" max="8" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4273,2073 +3388,411 @@
         <v>7</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>476</v>
+        <v>190</v>
       </c>
       <c r="C2" s="2">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="2">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="2">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="2">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="2">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="2">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K2" t="s">
-        <v>404</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="C3" s="2">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="C4" s="2">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="J8" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="2">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="2">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K4" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C5" s="2">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K5" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C6" s="2">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K6" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="C7" s="2">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K7" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C8" s="2">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C9" s="2">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K9" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C10" s="2">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="I10" s="2" t="s">
-        <v>332</v>
+        <v>135</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K10" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="C11" s="2">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K11" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C12" s="2">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K12" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C13" s="2">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K13" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C14" s="2">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K14" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C15" s="2">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K15" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="C16" s="2">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K16" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C17" s="2">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K17" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C18" s="2">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C19" s="2">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K19" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C20" s="2">
-        <v>11</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K20" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C21" s="2">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K21" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C22" s="2">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K22" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="C23" s="2">
-        <v>15</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K23" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C24" s="2">
-        <v>11</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K24" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="C25" s="2">
-        <v>11</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K25" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C26" s="2">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K26" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C27" s="2">
-        <v>11</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K27" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C28" s="2">
-        <v>14</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K28" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C29" s="2">
-        <v>11</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K29" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C30" s="2">
-        <v>11</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K30" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C31" s="2">
-        <v>11</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K31" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C32" s="2">
-        <v>11</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K32" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C33" s="2">
-        <v>11</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K33" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C34" s="2">
-        <v>11</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K34" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="C35" s="2">
-        <v>11</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K35" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C36" s="2">
-        <v>11</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K36" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C37" s="2">
-        <v>11</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K37" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="C38" s="2">
-        <v>11</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K38" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C39" s="2">
-        <v>11</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K39" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C40" s="2">
-        <v>11</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K40" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C41" s="2">
-        <v>11</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="J41" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K41" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C42" s="2">
-        <v>11</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K42" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C43" s="2">
-        <v>11</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K43" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C44" s="2">
-        <v>11</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K44" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C45" s="2">
-        <v>11</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="J45" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K45" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C46" s="2">
-        <v>11</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="J46" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K46" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C47" s="2">
-        <v>11</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="J47" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K47" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C48" s="2">
-        <v>11</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K48" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C49" s="2">
-        <v>11</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J49" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K49" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C50" s="2">
-        <v>31</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K50" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C51" s="2">
-        <v>11</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="J51" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K51" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C52" s="2">
-        <v>11</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="J52" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K52" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C53" s="2">
-        <v>11</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J53" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K53" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C54" s="2">
-        <v>11</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K54" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="C55" s="2">
-        <v>11</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="J55" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K55" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C56" s="2">
-        <v>11</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="J56" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K56" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C57" s="2">
-        <v>11</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K57" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C58" s="2">
-        <v>11</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="J58" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K58" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
-    </row>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -7667,59 +5120,10 @@
     <row r="1389" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="1390" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="1391" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1392" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1393" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1394" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1395" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1396" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1397" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1398" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1399" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1400" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1401" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1402" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1403" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1404" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1405" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1406" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1407" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1408" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1409" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1410" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1411" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1412" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1413" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1414" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1415" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1416" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1417" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1418" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1419" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1420" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1421" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1422" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1423" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1424" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1425" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1426" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1427" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1428" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1429" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1430" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1431" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1432" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1433" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1434" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1435" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1436" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1437" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1438" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="1439" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{8416A06A-C38F-4887-AC07-D22F5F1B3185}"/>
-    <hyperlink ref="J2:J58" r:id="rId2" display="suporte.ti@unitaengenharia.com.br" xr:uid="{864D7787-F618-4BCE-9DA2-C37A81AA5D75}"/>
-  </hyperlinks>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J10">
+    <sortCondition ref="A1:A10"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>